<commit_message>
new topics and keywords
</commit_message>
<xml_diff>
--- a/flatfiles/topics.xlsx
+++ b/flatfiles/topics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uzinfocom/Desktop/LEXX/chat_bot/flatfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uzinfocom/Downloads/Telegram Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D6CB69-35A4-F147-B564-755C5E903693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6945F07-BC5D-1B4F-BD68-156274F7FC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Cтипендия</t>
   </si>
   <si>
-    <t>Психолог</t>
-  </si>
-  <si>
     <t>Каналы</t>
   </si>
   <si>
@@ -89,6 +86,36 @@
   </si>
   <si>
     <t>Организационная структура</t>
+  </si>
+  <si>
+    <t>Выплаты</t>
+  </si>
+  <si>
+    <t>Обратная связь</t>
+  </si>
+  <si>
+    <t>Риски</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Развитие </t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>коммуникации</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>NOOB</t>
+  </si>
+  <si>
+    <t>Result bot</t>
   </si>
 </sst>
 </file>
@@ -493,10 +520,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -596,10 +623,13 @@
       <c r="E5" s="5">
         <v>607979249</v>
       </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -614,12 +644,12 @@
         <v>607979249</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -632,9 +662,6 @@
       </c>
       <c r="E7" s="5">
         <v>607979249</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -655,7 +682,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -774,50 +801,157 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5">
+        <v>607979249</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5">
+        <v>607979249</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
@@ -869,11 +1003,6 @@
       <c r="C34" s="8"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="E35" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>